<commit_message>
Report plots and tables
</commit_message>
<xml_diff>
--- a/tabulatedData/table_users.xlsx
+++ b/tabulatedData/table_users.xlsx
@@ -1,93 +1,436 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView windowWidth="23175" windowHeight="9750"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
-    <t xml:space="preserve"/>
+    <t>State</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
+    <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">Média</t>
+    <t>Day Week</t>
   </si>
   <si>
-    <t xml:space="preserve">DesvioPadrão</t>
+    <t>Mean</t>
   </si>
   <si>
-    <t xml:space="preserve">Mínimo</t>
+    <t>SD</t>
   </si>
   <si>
-    <t xml:space="preserve">1Quartil</t>
+    <t>Min</t>
   </si>
   <si>
-    <t xml:space="preserve">Mediana</t>
+    <t>1st Quart.</t>
   </si>
   <si>
-    <t xml:space="preserve">3Quartil</t>
+    <t>Median</t>
   </si>
   <si>
-    <t xml:space="preserve">Máximo</t>
+    <t>3rd Quart.</t>
   </si>
   <si>
-    <t xml:space="preserve">RJ  2019  Weekday</t>
+    <t>Max</t>
   </si>
   <si>
-    <t xml:space="preserve">RJ  2019  Weekend</t>
+    <t>RJ</t>
   </si>
   <si>
-    <t xml:space="preserve">RJ  2020  Weekday</t>
+    <t>Weekday</t>
   </si>
   <si>
-    <t xml:space="preserve">RJ  2020  Weekend</t>
+    <t>Weekend</t>
   </si>
   <si>
-    <t xml:space="preserve">SP  2019  Weekday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP  2019  Weekend</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP  2020  Weekday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP  2020  Weekend</t>
+    <t>SP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="#,#00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -95,17 +438,353 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -382,281 +1061,309 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="J14:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="I11" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="5.3" customWidth="1"/>
+    <col min="3" max="3" width="5.1" customWidth="1"/>
+    <col min="4" max="6" width="4.7" customWidth="1"/>
+    <col min="7" max="7" width="4.9" customWidth="1"/>
+    <col min="8" max="8" width="4.7" customWidth="1"/>
+    <col min="9" max="9" width="5" customWidth="1"/>
+    <col min="10" max="10" width="4.7" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="14" spans="10:19">
+      <c r="J14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="K14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="R14" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="S14" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="n">
-        <v>21</v>
-      </c>
-      <c r="C2" t="n">
+    <row r="15" spans="10:19">
+      <c r="J15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2019</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="6">
         <v>1053615.38095238</v>
       </c>
-      <c r="D2" t="n">
+      <c r="N15" s="6">
         <v>259720.895133502</v>
       </c>
-      <c r="E2" t="n">
+      <c r="O15" s="6">
         <v>528805</v>
       </c>
-      <c r="F2" t="n">
+      <c r="P15" s="6">
         <v>790609</v>
       </c>
-      <c r="G2" t="n">
+      <c r="Q15" s="6">
         <v>1140444</v>
       </c>
-      <c r="H2" t="n">
+      <c r="R15" s="6">
         <v>1180351</v>
       </c>
-      <c r="I2" t="n">
+      <c r="S15" s="6">
         <v>1465666</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" t="n">
+    <row r="16" spans="10:19">
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="7">
         <v>938471.888888889</v>
       </c>
-      <c r="D3" t="n">
+      <c r="N16" s="7">
         <v>163672.141262223</v>
       </c>
-      <c r="E3" t="n">
+      <c r="O16" s="7">
         <v>679678</v>
       </c>
-      <c r="F3" t="n">
+      <c r="P16" s="7">
         <v>811883</v>
       </c>
-      <c r="G3" t="n">
+      <c r="Q16" s="7">
         <v>962988</v>
       </c>
-      <c r="H3" t="n">
+      <c r="R16" s="7">
         <v>1026558</v>
       </c>
-      <c r="I3" t="n">
+      <c r="S16" s="7">
         <v>1201777</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="17" spans="10:19">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3">
+        <v>2020</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="n">
-        <v>21</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="M17" s="6">
         <v>870919.904761905</v>
       </c>
-      <c r="D4" t="n">
+      <c r="N17" s="6">
         <v>445958.451765958</v>
       </c>
-      <c r="E4" t="n">
+      <c r="O17" s="6">
         <v>214521</v>
       </c>
-      <c r="F4" t="n">
+      <c r="P17" s="6">
         <v>509431</v>
       </c>
-      <c r="G4" t="n">
+      <c r="Q17" s="6">
         <v>870189</v>
       </c>
-      <c r="H4" t="n">
+      <c r="R17" s="6">
         <v>1196752</v>
       </c>
-      <c r="I4" t="n">
+      <c r="S17" s="6">
         <v>1682386</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="18" spans="10:19">
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="n">
-        <v>9</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="M18" s="7">
         <v>624417.333333333</v>
       </c>
-      <c r="D5" t="n">
+      <c r="N18" s="7">
         <v>425257.561164114</v>
       </c>
-      <c r="E5" t="n">
+      <c r="O18" s="7">
         <v>179309</v>
       </c>
-      <c r="F5" t="n">
+      <c r="P18" s="7">
         <v>238466</v>
       </c>
-      <c r="G5" t="n">
+      <c r="Q18" s="7">
         <v>442211</v>
       </c>
-      <c r="H5" t="n">
+      <c r="R18" s="7">
         <v>1023705</v>
       </c>
-      <c r="I5" t="n">
+      <c r="S18" s="7">
         <v>1332701</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="19" spans="10:19">
+      <c r="J19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="K19" s="3">
+        <v>2019</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="6">
         <v>3708275.76190476</v>
       </c>
-      <c r="D6" t="n">
+      <c r="N19" s="6">
         <v>850838.702512697</v>
       </c>
-      <c r="E6" t="n">
+      <c r="O19" s="6">
         <v>2221510</v>
       </c>
-      <c r="F6" t="n">
+      <c r="P19" s="6">
         <v>2790522</v>
       </c>
-      <c r="G6" t="n">
+      <c r="Q19" s="6">
         <v>3927577</v>
       </c>
-      <c r="H6" t="n">
+      <c r="R19" s="6">
         <v>4169805</v>
       </c>
-      <c r="I6" t="n">
+      <c r="S19" s="6">
         <v>5011449</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
+    <row r="20" spans="10:19">
+      <c r="J20" s="3"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="7">
         <v>3256168.77777778</v>
       </c>
-      <c r="D7" t="n">
+      <c r="N20" s="7">
         <v>563221.813569214</v>
       </c>
-      <c r="E7" t="n">
+      <c r="O20" s="7">
         <v>2456231</v>
       </c>
-      <c r="F7" t="n">
+      <c r="P20" s="7">
         <v>2756478</v>
       </c>
-      <c r="G7" t="n">
+      <c r="Q20" s="7">
         <v>3550141</v>
       </c>
-      <c r="H7" t="n">
+      <c r="R20" s="7">
         <v>3569211</v>
       </c>
-      <c r="I7" t="n">
+      <c r="S20" s="7">
         <v>4172801</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="n">
-        <v>21</v>
-      </c>
-      <c r="C8" t="n">
+    <row r="21" spans="10:19">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>2020</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M21" s="6">
         <v>4353781.95238095</v>
       </c>
-      <c r="D8" t="n">
+      <c r="N21" s="6">
         <v>1652625.33826181</v>
       </c>
-      <c r="E8" t="n">
+      <c r="O21" s="6">
         <v>1661284</v>
       </c>
-      <c r="F8" t="n">
+      <c r="P21" s="6">
         <v>2816090</v>
       </c>
-      <c r="G8" t="n">
+      <c r="Q21" s="6">
         <v>4465741</v>
       </c>
-      <c r="H8" t="n">
+      <c r="R21" s="6">
         <v>5545852</v>
       </c>
-      <c r="I8" t="n">
+      <c r="S21" s="6">
         <v>7384012</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" t="n">
+    <row r="22" spans="10:19">
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="7">
         <v>3561948.88888889</v>
       </c>
-      <c r="D9" t="n">
+      <c r="N22" s="7">
         <v>1495901.96479444</v>
       </c>
-      <c r="E9" t="n">
+      <c r="O22" s="7">
         <v>1681135</v>
       </c>
-      <c r="F9" t="n">
+      <c r="P22" s="7">
         <v>2118311</v>
       </c>
-      <c r="G9" t="n">
+      <c r="Q22" s="7">
         <v>3964115</v>
       </c>
-      <c r="H9" t="n">
+      <c r="R22" s="7">
         <v>4999465</v>
       </c>
-      <c r="I9" t="n">
+      <c r="S22" s="7">
         <v>5527734</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="J19:J22"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="K21:K22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>